<commit_message>
added ppx presentation + underlined best values in .xlsx
</commit_message>
<xml_diff>
--- a/results/metrics_summary_all_conditions.xlsx
+++ b/results/metrics_summary_all_conditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuse\Desktop\cartella_informatica\magistrale\imaging\TomographicReconstruction\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ma3ti/Documents/Uni/Magistrale/Computational_imaging/TomographicReconstruction/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010AC955-AED8-4FE1-94AF-72E9CBB190C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA82D10-4045-7748-A190-3721129A1CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="36000" windowHeight="22520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -755,14 +755,21 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -792,14 +799,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1101,29 +1109,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" customWidth="1"/>
+    <col min="12" max="12" width="15.5" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1173,7 +1182,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1223,7 +1232,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1260,7 +1269,7 @@
       <c r="L3" t="s">
         <v>39</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N3" t="s">
@@ -1269,11 +1278,11 @@
       <c r="O3" t="s">
         <v>42</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1286,44 +1295,44 @@
       <c r="D4">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="2" t="s">
         <v>52</v>
       </c>
       <c r="M4" t="s">
         <v>53</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="2" t="s">
         <v>55</v>
       </c>
       <c r="P4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1373,7 +1382,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1392,7 +1401,7 @@
       <c r="F7" t="s">
         <v>71</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>72</v>
       </c>
       <c r="H7" t="s">
@@ -1423,7 +1432,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -1436,44 +1445,44 @@
       <c r="D8">
         <v>20</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>83</v>
       </c>
       <c r="G8" t="s">
         <v>84</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O8" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1523,7 +1532,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1560,7 +1569,7 @@
       <c r="L11" t="s">
         <v>114</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="2" t="s">
         <v>115</v>
       </c>
       <c r="N11" t="s">
@@ -1569,11 +1578,11 @@
       <c r="O11" t="s">
         <v>117</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1586,44 +1595,44 @@
       <c r="D12">
         <v>20</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="2" t="s">
         <v>126</v>
       </c>
       <c r="M12" t="s">
         <v>127</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12" s="2" t="s">
         <v>129</v>
       </c>
       <c r="P12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1673,7 +1682,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1695,7 +1704,7 @@
       <c r="G15" t="s">
         <v>145</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="2" t="s">
         <v>146</v>
       </c>
       <c r="I15" t="s">
@@ -1723,7 +1732,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1736,44 +1745,44 @@
       <c r="D16">
         <v>20</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="2" t="s">
         <v>157</v>
       </c>
       <c r="H16" t="s">
         <v>158</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N16" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O16" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="P16" t="s">
+      <c r="P16" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1823,7 +1832,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1836,44 +1845,44 @@
       <c r="D19">
         <v>20</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
         <v>189</v>
       </c>
       <c r="G19" t="s">
         <v>188</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M19" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N19" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="O19" t="s">
+      <c r="O19" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="P19" t="s">
+      <c r="P19" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1892,7 +1901,7 @@
       <c r="F20" t="s">
         <v>201</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="2" t="s">
         <v>200</v>
       </c>
       <c r="H20" t="s">
@@ -1923,7 +1932,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1973,7 +1982,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -2023,7 +2032,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -2036,40 +2045,40 @@
       <c r="D24">
         <v>20</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M24" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="N24" t="s">
+      <c r="N24" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="O24" t="s">
+      <c r="O24" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P24" s="2" t="s">
         <v>227</v>
       </c>
     </row>

</xml_diff>